<commit_message>
feat: Introduced dynamic Excel-driven UI with sheet switching and adaptive data entry
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -472,6 +472,36 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>aa</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>5</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>tepong32@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>aa         a</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>33</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>tepong32@gmail.com</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
the app now works as an excel reader with input validations in place and better UI. see changelogs for more info.
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -502,6 +502,81 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>a f f asdf a</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>3</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>teppy@teppy.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>asdf asdf</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>12</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>te@ttp.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>asdf ththth gh</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>12</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>asdf@adfas.cc</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>asdf</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>2</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>asdf@fga.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>saasd asdfasd</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>12</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>sadf@gds.com</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
added duplicate checker thru header tags (unique) or 'ID' on it.
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -562,21 +562,6 @@
         </is>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>saasd asdfasd</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>12</v>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>sadf@gds.com</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>